<commit_message>
Define the date column width of zdemo_excel10
</commit_message>
<xml_diff>
--- a/src/zdemo_excel10.w3mi.data.xlsx
+++ b/src/zdemo_excel10.w3mi.data.xlsx
@@ -372,10 +372,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:outlineLevelCol="0"/>
   <cols>
-    <col min="4" max="4" width="1.3000000000000000E+01" customWidth="true"/>
+    <col min="2" max="2" width="1.7000000000000000E+01" customWidth="true"/>
     <col min="1" max="1" width="9.10"/>
-    <col min="2" max="2" width="9.10"/>
     <col min="3" max="3" width="9.10"/>
+    <col min="4" max="4" width="9.10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>

<commit_message>
Set column width via field catalog (#64)
* Define the date column width of zdemo_excel10
</commit_message>
<xml_diff>
--- a/src/zdemo_excel10.w3mi.data.xlsx
+++ b/src/zdemo_excel10.w3mi.data.xlsx
@@ -372,10 +372,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:outlineLevelCol="0"/>
   <cols>
-    <col min="4" max="4" width="1.3000000000000000E+01" customWidth="true"/>
+    <col min="2" max="2" width="1.3000000000000000E+01" customWidth="true"/>
     <col min="1" max="1" width="9.10"/>
-    <col min="2" max="2" width="9.10"/>
     <col min="3" max="3" width="9.10"/>
+    <col min="4" max="4" width="9.10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>